<commit_message>
Complete Optimization Code Works for 2 Stages
</commit_message>
<xml_diff>
--- a/SRM Sizing/InputOutput.xlsx
+++ b/SRM Sizing/InputOutput.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,13 +10,13 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="294" documentId="8_{C7C79824-C540-4E01-B25D-0EC6B092111C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F767C21B-D6DB-4B72-9D3B-702165C4EB18}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Graph Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -111,18 +111,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.5999938962981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="-0.24997711111789"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -145,49 +145,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" justifyLastLine="false" shrinkToFit="false" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" justifyLastLine="false" shrinkToFit="false" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" justifyLastLine="false" shrinkToFit="false" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" justifyLastLine="false" shrinkToFit="false" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -203,46 +205,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{632FF417-F36D-4731-8894-50278695E809}" name="Table1" displayName="Table1" ref="A2:B77" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" id="1" name="Table1" displayName="Table1" ref="A2:B77" totalsRowShown="false" headerRowDxfId="3" mc:Ignorable="xr xr3" xr:uid="{632FF417-F36D-4731-8894-50278695E809}">
   <autoFilter ref="A2:B77" xr:uid="{632FF417-F36D-4731-8894-50278695E809}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{071ACD4F-1829-41DF-9655-E15F36E9FA8E}" name="Time"/>
-    <tableColumn id="2" xr3:uid="{429992EE-A094-4C72-9B77-CDB587F7B261}" name="Thrust"/>
+    <tableColumn id="1" name="Time" xr3:uid="{071ACD4F-1829-41DF-9655-E15F36E9FA8E}"/>
+    <tableColumn id="2" name="Thrust" xr3:uid="{429992EE-A094-4C72-9B77-CDB587F7B261}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C922686C-E97E-4E75-A61B-51104B514FAF}" name="Table2" displayName="Table2" ref="D2:E77" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" id="2" name="Table2" displayName="Table2" ref="D2:E77" totalsRowShown="false" headerRowDxfId="2" mc:Ignorable="xr xr3" xr:uid="{C922686C-E97E-4E75-A61B-51104B514FAF}">
   <autoFilter ref="D2:E77" xr:uid="{C922686C-E97E-4E75-A61B-51104B514FAF}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2D766A59-E644-4D95-BC4C-3EC2C3A72651}" name="Time"/>
-    <tableColumn id="2" xr3:uid="{29397DEC-0F32-43FC-A3E0-0EF286362D12}" name="Mass"/>
+    <tableColumn id="1" name="Time" xr3:uid="{2D766A59-E644-4D95-BC4C-3EC2C3A72651}"/>
+    <tableColumn id="2" name="Mass" xr3:uid="{29397DEC-0F32-43FC-A3E0-0EF286362D12}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{14492666-2012-45DD-AC98-4AC3A4944B07}" name="Table3" displayName="Table3" ref="G2:H77" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" id="3" name="Table3" displayName="Table3" ref="G2:H77" totalsRowShown="false" headerRowDxfId="1" mc:Ignorable="xr xr3" xr:uid="{14492666-2012-45DD-AC98-4AC3A4944B07}">
   <autoFilter ref="G2:H77" xr:uid="{14492666-2012-45DD-AC98-4AC3A4944B07}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7A06F39E-F04E-4540-907F-A857CF804039}" name="Time"/>
-    <tableColumn id="2" xr3:uid="{5E107804-2F4F-4351-91DD-FA4021AA9D08}" name="TTW Ratio"/>
+    <tableColumn id="1" name="Time" xr3:uid="{7A06F39E-F04E-4540-907F-A857CF804039}"/>
+    <tableColumn id="2" name="TTW Ratio" xr3:uid="{5E107804-2F4F-4351-91DD-FA4021AA9D08}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7D056DBF-34B0-4585-9077-0D50B6362AE0}" name="Table4" displayName="Table4" ref="J2:K77" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" id="4" name="Table4" displayName="Table4" ref="J2:K77" totalsRowShown="false" headerRowDxfId="0" mc:Ignorable="xr xr3" xr:uid="{7D056DBF-34B0-4585-9077-0D50B6362AE0}">
   <autoFilter ref="J2:K77" xr:uid="{7D056DBF-34B0-4585-9077-0D50B6362AE0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C0204B9B-A974-4964-BFFB-6865CFEDBAF6}" name="Time"/>
-    <tableColumn id="2" xr3:uid="{72E1B78D-A0F3-4977-9D91-8C8DA68A8BE6}" name="Pressure"/>
+    <tableColumn id="1" name="Time" xr3:uid="{C0204B9B-A974-4964-BFFB-6865CFEDBAF6}"/>
+    <tableColumn id="2" name="Pressure" xr3:uid="{72E1B78D-A0F3-4977-9D91-8C8DA68A8BE6}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
 </table>
 </file>
 
@@ -545,26 +547,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0EEA0E-8733-4844-A75F-4B4160C3709A}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="2.40625" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="3" width="3.2265625" customWidth="1"/>
-    <col min="4" max="4" width="12.2265625" customWidth="1"/>
-    <col min="5" max="5" width="2.953125" customWidth="1"/>
-    <col min="6" max="6" width="16.6796875" customWidth="1"/>
-    <col min="7" max="7" width="2.54296875" customWidth="1"/>
-    <col min="8" max="8" width="17.04296875" customWidth="1"/>
-    <col min="9" max="9" width="2.1796875" customWidth="1"/>
-    <col min="10" max="10" width="13.04296875" customWidth="1"/>
-    <col min="11" max="11" width="2.453125" customWidth="1"/>
+    <col min="1" max="1" width="2.40625" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="3.2265625" customWidth="true"/>
+    <col min="4" max="4" width="10.7109375" customWidth="true"/>
+    <col min="5" max="5" width="2.953125" customWidth="true"/>
+    <col min="6" max="6" width="4.7109375" customWidth="true"/>
+    <col min="7" max="7" width="2.54296875" customWidth="true"/>
+    <col min="8" max="8" width="3.15625" customWidth="true"/>
+    <col min="9" max="9" width="2.1796875" customWidth="true"/>
+    <col min="10" max="10" width="7.7109375" customWidth="true"/>
+    <col min="11" max="11" width="2.453125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="1" x14ac:dyDescent="0.75">
       <c r="A1" s="5"/>
       <c r="B1" s="9" t="s">
         <v>9</v>
@@ -605,17 +607,27 @@
       <c r="Z1" s="15"/>
       <c r="AA1" s="15"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="2" x14ac:dyDescent="0.75">
       <c r="A2" s="5"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="11">
+        <v>5785.6263429175469</v>
+      </c>
       <c r="C2" s="8"/>
-      <c r="D2" s="12"/>
+      <c r="D2" s="12">
+        <v>27.509567499970444</v>
+      </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="12"/>
+      <c r="F2" s="12">
+        <v>0.14999999999999999</v>
+      </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="12">
+        <v>10</v>
+      </c>
       <c r="I2" s="6"/>
-      <c r="J2" s="12"/>
+      <c r="J2" s="12">
+        <v>0.0022499999999999998</v>
+      </c>
       <c r="K2" s="6"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -626,17 +638,27 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="3" x14ac:dyDescent="0.75">
       <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
+      <c r="B3" s="11">
+        <v>6000.8168203639143</v>
+      </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="12"/>
+      <c r="D3" s="12">
+        <v>24.049923240085576</v>
+      </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="12"/>
+      <c r="F3" s="12">
+        <v>0.14999999999999999</v>
+      </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="12">
+        <v>10</v>
+      </c>
       <c r="I3" s="6"/>
-      <c r="J3" s="12"/>
+      <c r="J3" s="12">
+        <v>0.059999999999999998</v>
+      </c>
       <c r="K3" s="6"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -647,7 +669,7 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="4" x14ac:dyDescent="0.75">
       <c r="A4" s="5"/>
       <c r="B4" s="11"/>
       <c r="C4" s="8"/>
@@ -668,7 +690,7 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="5" x14ac:dyDescent="0.75">
       <c r="A5" s="5"/>
       <c r="B5" s="11"/>
       <c r="C5" s="8"/>
@@ -689,7 +711,7 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="6" x14ac:dyDescent="0.75">
       <c r="A6" s="5"/>
       <c r="B6" s="11"/>
       <c r="C6" s="8"/>
@@ -702,7 +724,7 @@
       <c r="J6" s="14"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="7" x14ac:dyDescent="0.75">
       <c r="A7" s="5"/>
       <c r="B7" s="11"/>
       <c r="C7" s="8"/>
@@ -715,7 +737,7 @@
       <c r="J7" s="14"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="8" x14ac:dyDescent="0.75">
       <c r="A8" s="5"/>
       <c r="B8" s="11"/>
       <c r="C8" s="8"/>
@@ -728,7 +750,7 @@
       <c r="J8" s="14"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="9" x14ac:dyDescent="0.75">
       <c r="A9" s="5"/>
       <c r="B9" s="11"/>
       <c r="C9" s="8"/>
@@ -741,7 +763,7 @@
       <c r="J9" s="14"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="10" x14ac:dyDescent="0.75">
       <c r="A10" s="5"/>
       <c r="B10" s="11"/>
       <c r="C10" s="8"/>
@@ -754,7 +776,7 @@
       <c r="J10" s="14"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="11" x14ac:dyDescent="0.75">
       <c r="A11" s="5"/>
       <c r="B11" s="11"/>
       <c r="C11" s="8"/>
@@ -767,7 +789,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="12" x14ac:dyDescent="0.75">
       <c r="A12" s="5"/>
       <c r="B12" s="11"/>
       <c r="C12" s="8"/>
@@ -780,7 +802,7 @@
       <c r="J12" s="14"/>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="13" x14ac:dyDescent="0.75">
       <c r="A13" s="6"/>
       <c r="B13" s="12"/>
       <c r="C13" s="6"/>
@@ -793,7 +815,7 @@
       <c r="J13" s="14"/>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="14" x14ac:dyDescent="0.75">
       <c r="A14" s="6"/>
       <c r="B14" s="12"/>
       <c r="C14" s="6"/>
@@ -806,7 +828,7 @@
       <c r="J14" s="14"/>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="15" x14ac:dyDescent="0.75">
       <c r="A15" s="7"/>
       <c r="B15" s="11"/>
       <c r="C15" s="7"/>
@@ -819,7 +841,7 @@
       <c r="J15" s="14"/>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.75">
+    <row r="16" x14ac:dyDescent="0.75">
       <c r="A16" s="7"/>
       <c r="B16" s="13"/>
       <c r="C16" s="7"/>
@@ -832,7 +854,7 @@
       <c r="J16" s="14"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="17" x14ac:dyDescent="0.75">
       <c r="A17" s="7"/>
       <c r="B17" s="13"/>
       <c r="C17" s="7"/>
@@ -845,7 +867,7 @@
       <c r="J17" s="14"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="18" x14ac:dyDescent="0.75">
       <c r="A18" s="7"/>
       <c r="B18" s="13"/>
       <c r="C18" s="7"/>
@@ -858,7 +880,7 @@
       <c r="J18" s="14"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="19" x14ac:dyDescent="0.75">
       <c r="A19" s="7"/>
       <c r="B19" s="13"/>
       <c r="C19" s="7"/>
@@ -871,7 +893,7 @@
       <c r="J19" s="14"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="20" x14ac:dyDescent="0.75">
       <c r="A20" s="7"/>
       <c r="B20" s="13"/>
       <c r="C20" s="7"/>
@@ -884,7 +906,7 @@
       <c r="J20" s="14"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="21" x14ac:dyDescent="0.75">
       <c r="A21" s="7"/>
       <c r="B21" s="13"/>
       <c r="C21" s="7"/>
@@ -897,7 +919,7 @@
       <c r="J21" s="14"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="22" x14ac:dyDescent="0.75">
       <c r="A22" s="7"/>
       <c r="B22" s="13"/>
       <c r="C22" s="7"/>
@@ -910,7 +932,7 @@
       <c r="J22" s="14"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="23" x14ac:dyDescent="0.75">
       <c r="A23" s="7"/>
       <c r="B23" s="13"/>
       <c r="C23" s="7"/>
@@ -923,7 +945,7 @@
       <c r="J23" s="14"/>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="24" x14ac:dyDescent="0.75">
       <c r="A24" s="7"/>
       <c r="B24" s="13"/>
       <c r="C24" s="7"/>
@@ -936,7 +958,7 @@
       <c r="J24" s="14"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="25" x14ac:dyDescent="0.75">
       <c r="A25" s="7"/>
       <c r="B25" s="13"/>
       <c r="C25" s="7"/>
@@ -949,7 +971,7 @@
       <c r="J25" s="14"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="26" x14ac:dyDescent="0.75">
       <c r="A26" s="7"/>
       <c r="B26" s="13"/>
       <c r="C26" s="7"/>
@@ -962,7 +984,7 @@
       <c r="J26" s="14"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="27" x14ac:dyDescent="0.75">
       <c r="A27" s="7"/>
       <c r="B27" s="13"/>
       <c r="C27" s="7"/>
@@ -975,7 +997,7 @@
       <c r="J27" s="14"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="28" x14ac:dyDescent="0.75">
       <c r="A28" s="7"/>
       <c r="B28" s="13"/>
       <c r="C28" s="7"/>
@@ -988,7 +1010,7 @@
       <c r="J28" s="14"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="29" x14ac:dyDescent="0.75">
       <c r="A29" s="6"/>
       <c r="B29" s="14"/>
       <c r="C29" s="6"/>
@@ -1001,7 +1023,7 @@
       <c r="J29" s="14"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="30" x14ac:dyDescent="0.75">
       <c r="A30" s="6"/>
       <c r="B30" s="14"/>
       <c r="C30" s="6"/>
@@ -1014,7 +1036,7 @@
       <c r="J30" s="14"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="31" x14ac:dyDescent="0.75">
       <c r="A31" s="6"/>
       <c r="B31" s="14"/>
       <c r="C31" s="6"/>
@@ -1027,7 +1049,7 @@
       <c r="J31" s="14"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="32" x14ac:dyDescent="0.75">
       <c r="B32" s="2"/>
     </row>
   </sheetData>
@@ -1049,17 +1071,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="6.36328125" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" customWidth="1"/>
-    <col min="5" max="5" width="5.40625" customWidth="1"/>
-    <col min="7" max="7" width="5.1796875" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" customWidth="1"/>
-    <col min="10" max="10" width="5.1796875" customWidth="1"/>
-    <col min="11" max="11" width="8.1796875" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="true"/>
+    <col min="2" max="2" width="6.36328125" customWidth="true"/>
+    <col min="4" max="4" width="5.1796875" customWidth="true"/>
+    <col min="5" max="5" width="5.40625" customWidth="true"/>
+    <col min="7" max="7" width="5.1796875" customWidth="true"/>
+    <col min="8" max="8" width="9.54296875" customWidth="true"/>
+    <col min="10" max="10" width="5.1796875" customWidth="true"/>
+    <col min="11" max="11" width="8.1796875" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="1" x14ac:dyDescent="0.75">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="D1" s="3" t="s">
@@ -1075,7 +1097,7 @@
       </c>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="2" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1101,7 +1123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="3" x14ac:dyDescent="0.75">
       <c r="A3" s="1">
         <v>14</v>
       </c>
@@ -1127,7 +1149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="4" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Added Notes on minimum altitude and variable for minimum altitude
</commit_message>
<xml_diff>
--- a/SRM Sizing/InputOutput.xlsx
+++ b/SRM Sizing/InputOutput.xlsx
@@ -122,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -146,11 +146,16 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -174,6 +179,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,15 +564,15 @@
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="2.40625" customWidth="true"/>
-    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="2" max="2" width="11.60546875" customWidth="true"/>
     <col min="3" max="3" width="3.2265625" customWidth="true"/>
-    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="11.60546875" customWidth="true"/>
     <col min="5" max="5" width="2.953125" customWidth="true"/>
-    <col min="6" max="6" width="4.7109375" customWidth="true"/>
+    <col min="6" max="6" width="4.60546875" customWidth="true"/>
     <col min="7" max="7" width="2.54296875" customWidth="true"/>
-    <col min="8" max="8" width="4.7109375" customWidth="true"/>
+    <col min="8" max="8" width="3.60546875" customWidth="true"/>
     <col min="9" max="9" width="2.1796875" customWidth="true"/>
-    <col min="10" max="10" width="6.7109375" customWidth="true"/>
+    <col min="10" max="10" width="7.60546875" customWidth="true"/>
     <col min="11" max="11" width="2.453125" customWidth="true"/>
   </cols>
   <sheetData>
@@ -610,23 +620,23 @@
     <row r="2" x14ac:dyDescent="0.75">
       <c r="A2" s="5"/>
       <c r="B2" s="11">
-        <v>5585.4794408810758</v>
+        <v>5182.9191594237154</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="12">
-        <v>45.653570407933053</v>
+        <v>95.551444315269052</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="12">
-        <v>0.12</v>
+        <v>0.14999999999999999</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="12">
-        <v>2.75</v>
+        <v>3.5</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="12">
-        <v>0.0018</v>
+        <v>0.0022499999999999998</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="4"/>
@@ -641,23 +651,23 @@
     <row r="3" x14ac:dyDescent="0.75">
       <c r="A3" s="5"/>
       <c r="B3" s="11">
-        <v>5876.5198212818404</v>
+        <v>5301.2283828367363</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="12">
-        <v>41.858603589317717</v>
+        <v>84.553886601672104</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="12">
-        <v>0.12</v>
+        <v>0.14999999999999999</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="12">
-        <v>2.75</v>
+        <v>3.5</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="12">
-        <v>0.048000000000000001</v>
+        <v>0.059999999999999998</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="4"/>

</xml_diff>

<commit_message>
Added sounding rocket analysis to optimize, added altitude and dynamic pressure filter, and changed example call
</commit_message>
<xml_diff>
--- a/SRM Sizing/InputOutput.xlsx
+++ b/SRM Sizing/InputOutput.xlsx
@@ -122,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -151,11 +151,26 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -184,6 +199,21 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,7 +585,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0EEA0E-8733-4844-A75F-4B4160C3709A}">
-  <dimension ref="A1:AA32"/>
+  <dimension ref="B1:L24"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="S46" sqref="S46"/>
@@ -564,15 +594,15 @@
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="2.40625" customWidth="true"/>
-    <col min="2" max="2" width="11.60546875" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
     <col min="3" max="3" width="3.2265625" customWidth="true"/>
-    <col min="4" max="4" width="11.60546875" customWidth="true"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
     <col min="5" max="5" width="2.953125" customWidth="true"/>
-    <col min="6" max="6" width="4.60546875" customWidth="true"/>
+    <col min="6" max="6" width="12.7109375" customWidth="true"/>
     <col min="7" max="7" width="2.54296875" customWidth="true"/>
-    <col min="8" max="8" width="3.60546875" customWidth="true"/>
+    <col min="8" max="8" width="12.7109375" customWidth="true"/>
     <col min="9" max="9" width="2.1796875" customWidth="true"/>
-    <col min="10" max="10" width="7.60546875" customWidth="true"/>
+    <col min="10" max="10" width="13.7109375" customWidth="true"/>
     <col min="11" max="11" width="2.453125" customWidth="true"/>
   </cols>
   <sheetData>
@@ -620,23 +650,23 @@
     <row r="2" x14ac:dyDescent="0.75">
       <c r="A2" s="5"/>
       <c r="B2" s="11">
-        <v>5182.9191594237154</v>
+        <v>11759.785829309487</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="12">
-        <v>95.551444315269052</v>
+        <v>106.41279805705868</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="12">
-        <v>0.14999999999999999</v>
+        <v>0.41111111111111109</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="12">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="12">
-        <v>0.0022499999999999998</v>
+        <v>0.056111111111111112</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="4"/>
@@ -651,23 +681,23 @@
     <row r="3" x14ac:dyDescent="0.75">
       <c r="A3" s="5"/>
       <c r="B3" s="11">
-        <v>5301.2283828367363</v>
+        <v>11291.361151544121</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="12">
-        <v>84.553886601672104</v>
+        <v>103.78071378040131</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="12">
-        <v>0.14999999999999999</v>
+        <v>0.41111111111111109</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="12">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="12">
-        <v>0.059999999999999998</v>
+        <v>0.092222222222222233</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="4"/>
@@ -682,23 +712,23 @@
     <row r="4" x14ac:dyDescent="0.75">
       <c r="A4" s="5"/>
       <c r="B4" s="11">
-        <v>5152.2275417142437</v>
+        <v>10470.122444288485</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="12">
-        <v>3.0595568442353311</v>
+        <v>99.446667740395412</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="12">
-        <v>0.083999999999999991</v>
+        <v>0.41111111111111109</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="12">
-        <v>2.75</v>
+        <v>0.5</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="12">
-        <v>0.02282</v>
+        <v>0.12833333333333333</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="4"/>
@@ -713,23 +743,23 @@
     <row r="5" x14ac:dyDescent="0.75">
       <c r="A5" s="5"/>
       <c r="B5" s="11">
-        <v>5134.6479555732258</v>
+        <v>9388.711509950539</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="12">
-        <v>2.8985943709396089</v>
+        <v>93.275616648743764</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="12">
-        <v>0.083999999999999991</v>
+        <v>0.41111111111111109</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="12">
-        <v>2.75</v>
+        <v>0.5</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="12">
-        <v>0.033599999999999998</v>
+        <v>0.16444444444444445</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="4"/>
@@ -744,408 +774,438 @@
     <row r="6" x14ac:dyDescent="0.75">
       <c r="A6" s="5"/>
       <c r="B6" s="11">
-        <v>4678.3971750324126</v>
+        <v>14134.988085788713</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="12">
-        <v>2.6368678643384538</v>
+        <v>149.54913929186611</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="14">
-        <v>0.083999999999999991</v>
+        <v>0.4555555555555556</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="14">
-        <v>1.9249999999999998</v>
+        <v>0.57894736842105265</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="14">
-        <v>0.0012599999999999998</v>
+        <v>0.060555555555555571</v>
       </c>
       <c r="K6" s="6"/>
     </row>
     <row r="7" x14ac:dyDescent="0.75">
       <c r="A7" s="5"/>
       <c r="B7" s="11">
-        <v>4710.9752275043375</v>
+        <v>12980.866214258087</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="12">
-        <v>2.6103070591916406</v>
+        <v>144.79015560345718</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="14">
-        <v>0.083999999999999991</v>
+        <v>0.4555555555555556</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="14">
-        <v>1.9249999999999998</v>
+        <v>0.57894736842105265</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="14">
-        <v>0.012039999999999999</v>
+        <v>0.10111111111111114</v>
       </c>
       <c r="K7" s="6"/>
     </row>
     <row r="8" x14ac:dyDescent="0.75">
       <c r="A8" s="5"/>
       <c r="B8" s="11">
-        <v>4770.9233667570088</v>
+        <v>12039.356048207716</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="12">
-        <v>2.5406897909647341</v>
+        <v>138.79329792775252</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="14">
-        <v>0.083999999999999991</v>
+        <v>0.4555555555555556</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="14">
-        <v>1.9249999999999998</v>
+        <v>0.57894736842105265</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="14">
-        <v>0.02282</v>
+        <v>0.14166666666666669</v>
       </c>
       <c r="K8" s="6"/>
     </row>
     <row r="9" x14ac:dyDescent="0.75">
       <c r="A9" s="5"/>
       <c r="B9" s="11">
-        <v>4732.9979047061306</v>
+        <v>10866.829258794471</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="12">
-        <v>2.4280160596577254</v>
+        <v>130.6145859984448</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="14">
-        <v>0.083999999999999991</v>
+        <v>0.4555555555555556</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="14">
-        <v>1.9249999999999998</v>
+        <v>0.57894736842105265</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="14">
-        <v>0.033599999999999998</v>
+        <v>0.18222222222222226</v>
       </c>
       <c r="K9" s="6"/>
     </row>
     <row r="10" x14ac:dyDescent="0.75">
       <c r="A10" s="5"/>
       <c r="B10" s="11">
-        <v>5661.135994605138</v>
+        <v>12637.179893923547</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="12">
-        <v>5.1401103916573021</v>
+        <v>129.8378930247934</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="14">
-        <v>0.12</v>
+        <v>0.4555555555555556</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="14">
-        <v>2.75</v>
+        <v>0.5</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="14">
-        <v>0.0018</v>
+        <v>0.060555555555555571</v>
       </c>
       <c r="K10" s="6"/>
     </row>
     <row r="11" x14ac:dyDescent="0.75">
       <c r="A11" s="5"/>
       <c r="B11" s="11">
-        <v>5693.0317999837825</v>
+        <v>11989.332423696373</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="12">
-        <v>5.0626736419581349</v>
+        <v>125.72786165753115</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="14">
-        <v>0.12</v>
+        <v>0.4555555555555556</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="14">
-        <v>2.75</v>
+        <v>0.5</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="14">
-        <v>0.0172</v>
+        <v>0.10111111111111114</v>
       </c>
       <c r="K11" s="6"/>
     </row>
     <row r="12" x14ac:dyDescent="0.75">
       <c r="A12" s="5"/>
       <c r="B12" s="11">
-        <v>5800.320475297578</v>
+        <v>11145.832517634875</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="12">
-        <v>4.8597078453782245</v>
+        <v>120.54875730124078</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="14">
-        <v>0.12</v>
+        <v>0.4555555555555556</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="14">
-        <v>2.75</v>
+        <v>0.5</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="14">
-        <v>0.032599999999999997</v>
+        <v>0.14166666666666669</v>
       </c>
       <c r="K12" s="6"/>
     </row>
     <row r="13" x14ac:dyDescent="0.75">
       <c r="A13" s="6"/>
       <c r="B13" s="12">
-        <v>5867.1521530975779</v>
+        <v>10075.337559220534</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="12">
-        <v>4.531213001917564</v>
+        <v>113.48532427138412</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="14">
-        <v>0.12</v>
+        <v>0.4555555555555556</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="14">
-        <v>2.75</v>
+        <v>0.5</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="14">
-        <v>0.048000000000000001</v>
+        <v>0.18222222222222226</v>
       </c>
       <c r="K13" s="6"/>
     </row>
     <row r="14" x14ac:dyDescent="0.75">
       <c r="A14" s="6"/>
       <c r="B14" s="12">
-        <v>5414.0342296409599</v>
+        <v>18140.034242756843</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="12">
-        <v>3.9970772741601088</v>
+        <v>203.28065187582757</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="14">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="14">
-        <v>1.9249999999999998</v>
+        <v>0.65789473684210531</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="14">
-        <v>0.0018</v>
+        <v>0.065000000000000002</v>
       </c>
       <c r="K14" s="6"/>
     </row>
     <row r="15" x14ac:dyDescent="0.75">
       <c r="A15" s="7"/>
       <c r="B15" s="11">
-        <v>5449.0054978912649</v>
+        <v>16643.231958071461</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="11">
-        <v>3.9428715493706967</v>
+        <v>197.41227693867586</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="14">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="14">
-        <v>1.9249999999999998</v>
+        <v>0.65789473684210531</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="14">
-        <v>0.0172</v>
+        <v>0.11000000000000001</v>
       </c>
       <c r="K15" s="6"/>
     </row>
     <row r="16" x14ac:dyDescent="0.75">
       <c r="A16" s="7"/>
       <c r="B16" s="13">
-        <v>5542.8263499360228</v>
+        <v>13910.661919395623</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="13">
-        <v>3.800795491764756</v>
+        <v>187.55801847709702</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="14">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="14">
-        <v>1.9249999999999998</v>
+        <v>0.65789473684210531</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="14">
-        <v>0.032599999999999997</v>
+        <v>0.155</v>
       </c>
       <c r="K16" s="6"/>
     </row>
     <row r="17" x14ac:dyDescent="0.75">
       <c r="A17" s="7"/>
       <c r="B17" s="13">
-        <v>5590.1936868867197</v>
+        <v>15688.339757661297</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="13">
-        <v>3.5708491013422972</v>
+        <v>179.48697365072829</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="14">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="14">
-        <v>1.9249999999999998</v>
+        <v>0.57894736842105265</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="14">
-        <v>0.048000000000000001</v>
+        <v>0.065000000000000002</v>
       </c>
       <c r="K17" s="6"/>
     </row>
     <row r="18" x14ac:dyDescent="0.75">
       <c r="A18" s="7"/>
       <c r="B18" s="13">
-        <v>4915.8246352837195</v>
+        <v>14407.250779755384</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="13">
-        <v>2.8540441566629227</v>
+        <v>174.32280370603479</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="14">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="14">
-        <v>1.0999999999999999</v>
+        <v>0.57894736842105265</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="14">
-        <v>0.0018</v>
+        <v>0.11000000000000001</v>
       </c>
       <c r="K18" s="6"/>
     </row>
     <row r="19" x14ac:dyDescent="0.75">
       <c r="A19" s="7"/>
       <c r="B19" s="13">
-        <v>4943.7555940469892</v>
+        <v>12790.523914086445</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="13">
-        <v>2.823069456783255</v>
+        <v>165.65105625984543</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="14">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="14">
-        <v>1.0999999999999999</v>
+        <v>0.57894736842105265</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="14">
-        <v>0.0172</v>
+        <v>0.155</v>
       </c>
       <c r="K19" s="6"/>
     </row>
     <row r="20" x14ac:dyDescent="0.75">
       <c r="A20" s="7"/>
       <c r="B20" s="13">
-        <v>5013.2918606046251</v>
+        <v>11610.37514919874</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="13">
-        <v>2.7418831381512909</v>
+        <v>156.42302615529474</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="14">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="14">
-        <v>1.0999999999999999</v>
+        <v>0.57894736842105265</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="14">
-        <v>0.032599999999999997</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="K20" s="6"/>
     </row>
     <row r="21" x14ac:dyDescent="0.75">
       <c r="A21" s="7"/>
       <c r="B21" s="13">
-        <v>5027.3332118178969</v>
+        <v>13514.213697140234</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="13">
-        <v>2.6104852007670249</v>
+        <v>155.693295425629</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="14">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="14">
-        <v>1.0999999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="14">
-        <v>0.048000000000000001</v>
+        <v>0.065000000000000002</v>
       </c>
       <c r="K21" s="6"/>
     </row>
     <row r="22" x14ac:dyDescent="0.75">
       <c r="A22" s="7"/>
-      <c r="B22" s="13"/>
+      <c r="B22" s="13">
+        <v>12918.696413745649</v>
+      </c>
       <c r="C22" s="7"/>
-      <c r="D22" s="13"/>
+      <c r="D22" s="13">
+        <v>151.23333047339366</v>
+      </c>
       <c r="E22" s="6"/>
-      <c r="F22" s="14"/>
+      <c r="F22" s="14">
+        <v>0.5</v>
+      </c>
       <c r="G22" s="6"/>
-      <c r="H22" s="14"/>
+      <c r="H22" s="14">
+        <v>0.5</v>
+      </c>
       <c r="I22" s="6"/>
-      <c r="J22" s="14"/>
+      <c r="J22" s="14">
+        <v>0.11000000000000001</v>
+      </c>
       <c r="K22" s="6"/>
     </row>
     <row r="23" x14ac:dyDescent="0.75">
       <c r="A23" s="7"/>
-      <c r="B23" s="13"/>
+      <c r="B23" s="13">
+        <v>11804.118876785573</v>
+      </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="13"/>
+      <c r="D23" s="13">
+        <v>143.74409404259382</v>
+      </c>
       <c r="E23" s="6"/>
-      <c r="F23" s="14"/>
+      <c r="F23" s="14">
+        <v>0.5</v>
+      </c>
       <c r="G23" s="6"/>
-      <c r="H23" s="14"/>
+      <c r="H23" s="14">
+        <v>0.5</v>
+      </c>
       <c r="I23" s="6"/>
-      <c r="J23" s="14"/>
+      <c r="J23" s="14">
+        <v>0.155</v>
+      </c>
       <c r="K23" s="6"/>
     </row>
     <row r="24" x14ac:dyDescent="0.75">
       <c r="A24" s="7"/>
-      <c r="B24" s="13"/>
+      <c r="B24" s="13">
+        <v>10743.779107217671</v>
+      </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="13"/>
+      <c r="D24" s="13">
+        <v>135.77443167957273</v>
+      </c>
       <c r="E24" s="6"/>
-      <c r="F24" s="14"/>
+      <c r="F24" s="14">
+        <v>0.5</v>
+      </c>
       <c r="G24" s="6"/>
-      <c r="H24" s="14"/>
+      <c r="H24" s="14">
+        <v>0.5</v>
+      </c>
       <c r="I24" s="6"/>
-      <c r="J24" s="14"/>
+      <c r="J24" s="14">
+        <v>0.20000000000000001</v>
+      </c>
       <c r="K24" s="6"/>
     </row>
     <row r="25" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
Updated example call, removed dtFactor from altitude_analysis as it was unused, and changed initial web constraints in optimize
</commit_message>
<xml_diff>
--- a/SRM Sizing/InputOutput.xlsx
+++ b/SRM Sizing/InputOutput.xlsx
@@ -122,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -166,11 +166,21 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -214,6 +224,16 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>